<commit_message>
Added Details on scalar inverse
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91808\PycharmProjects\MULTIMODAL-FORECASTING-MODEL-FOR-STOCK-PRICE-PREDICTION-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52BA073F-053B-49DA-A262-37DA3F4429C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C987C1-67E1-427D-B74A-5750AF0DD0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7C42DFF4-176E-4CE1-9580-4A738A9BC40D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>ARIMA</t>
   </si>
@@ -69,6 +69,36 @@
   </si>
   <si>
     <t>Runtime</t>
+  </si>
+  <si>
+    <t>LSTM+Attention + ARIMA + GARCH</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Mamba</t>
+  </si>
+  <si>
+    <t>Arima + Garch</t>
+  </si>
+  <si>
+    <t>Arima + Garch + Sentiment Scores</t>
+  </si>
+  <si>
+    <t>Arima + Garch + Sentiment Scores + News vectors</t>
+  </si>
+  <si>
+    <t>N/a</t>
+  </si>
+  <si>
+    <t>Single Layer</t>
+  </si>
+  <si>
+    <t>Multilayer</t>
+  </si>
+  <si>
+    <t>Bidirectional</t>
   </si>
 </sst>
 </file>
@@ -84,12 +114,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,12 +146,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,27 +490,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BCEAEC-7ADE-4671-8EFD-C0FDDE92E385}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="1" max="8" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -495,74 +541,305 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2.4603199999999998</v>
+        <v>2.9986999999999999</v>
       </c>
       <c r="B7">
-        <v>1.56854</v>
+        <v>1.7310000000000001</v>
       </c>
       <c r="C7">
-        <v>1.6604000000000001</v>
+        <v>1.3789</v>
       </c>
       <c r="D7">
-        <v>0.90513999999999994</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E8">
-        <v>1</v>
+      <c r="A8">
+        <v>1.3533999999999999</v>
+      </c>
+      <c r="B8">
+        <v>1.1633</v>
+      </c>
+      <c r="C8">
+        <v>0.86629999999999996</v>
+      </c>
+      <c r="D8">
+        <v>0.94010000000000005</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3.9860000000000002</v>
+      </c>
+      <c r="B9">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="C9">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1">
+        <v>6.9444444444444448E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1.2999999999999999E-4</v>
+      </c>
+      <c r="B10">
+        <v>1.17E-2</v>
+      </c>
+      <c r="C10">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D10">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2.9986999999999999</v>
+      </c>
+      <c r="B16">
+        <v>1.7310000000000001</v>
+      </c>
+      <c r="C16">
+        <v>1.3789</v>
+      </c>
+      <c r="D16">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1.3533999999999999</v>
+      </c>
+      <c r="B17">
+        <v>1.1633</v>
+      </c>
+      <c r="C17">
+        <v>0.86629999999999996</v>
+      </c>
+      <c r="D17">
+        <v>0.94010000000000005</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2.9986999999999999</v>
+      </c>
+      <c r="B21">
+        <v>1.7310000000000001</v>
+      </c>
+      <c r="C21">
+        <v>1.3789</v>
+      </c>
+      <c r="D21">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1.3533999999999999</v>
+      </c>
+      <c r="B22">
+        <v>1.1633</v>
+      </c>
+      <c r="C22">
+        <v>0.86629999999999996</v>
+      </c>
+      <c r="D22">
+        <v>0.94010000000000005</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>